<commit_message>
Starting work on first alt
</commit_message>
<xml_diff>
--- a/CH-109 Custom Grouping.xlsx
+++ b/CH-109 Custom Grouping.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{98D61F39-7FD7-4B7C-B596-2B44FF8E61E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FB31DC-61DC-4C0A-B44D-8687DCAF2F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Original" sheetId="1" r:id="rId1"/>
+    <sheet name="Alt1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$2:$D$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Alt1'!$B$2:$D$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$D$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,8 +40,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
   <si>
     <t>Question</t>
   </si>
@@ -72,6 +96,9 @@
   </si>
   <si>
     <t>20/1/2024-24/1/2024</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/feed/update/urn:li:activity:7237927549903716352/</t>
   </si>
 </sst>
 </file>
@@ -905,12 +932,39 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="578" row="9">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{D98F7A14-C80F-4771-8AC1-A5AD72E9C885}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -933,6 +987,9 @@
         <v>1</v>
       </c>
       <c r="H1" s="35"/>
+      <c r="K1" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
@@ -1318,4 +1375,600 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F6C4476-87DA-43D4-910A-472BFDC6FEAE}">
+  <dimension ref="A1:N52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" customWidth="1"/>
+    <col min="4" max="5" width="12.21875" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" style="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="E1"/>
+      <c r="G1" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="35"/>
+      <c r="K1" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2"/>
+      <c r="G2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="16">
+        <v>45292</v>
+      </c>
+      <c r="C3" s="17">
+        <v>47</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3"/>
+      <c r="G3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="30">
+        <v>208</v>
+      </c>
+      <c r="I3" s="13"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="9"/>
+    </row>
+    <row r="4" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="16">
+        <v>45293</v>
+      </c>
+      <c r="C4" s="17">
+        <v>62</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4"/>
+      <c r="G4" s="12">
+        <v>45295</v>
+      </c>
+      <c r="H4" s="30">
+        <v>95</v>
+      </c>
+      <c r="I4" s="13"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="9"/>
+    </row>
+    <row r="5" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="16">
+        <v>45294</v>
+      </c>
+      <c r="C5" s="17">
+        <v>99</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5"/>
+      <c r="G5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="30">
+        <v>299</v>
+      </c>
+      <c r="I5" s="13"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="9"/>
+    </row>
+    <row r="6" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="12">
+        <v>45295</v>
+      </c>
+      <c r="C6" s="18">
+        <v>95</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6"/>
+      <c r="G6" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="30">
+        <v>303</v>
+      </c>
+      <c r="I6" s="13"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="9"/>
+    </row>
+    <row r="7" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="14">
+        <v>45296</v>
+      </c>
+      <c r="C7" s="15">
+        <v>52</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7"/>
+      <c r="G7" s="12">
+        <v>45303</v>
+      </c>
+      <c r="H7" s="30">
+        <v>101</v>
+      </c>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="14">
+        <v>45297</v>
+      </c>
+      <c r="C8" s="15">
+        <v>65</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8"/>
+      <c r="G8" s="12">
+        <v>45304</v>
+      </c>
+      <c r="H8" s="30">
+        <v>100</v>
+      </c>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+    </row>
+    <row r="9" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="14">
+        <v>45298</v>
+      </c>
+      <c r="C9" s="15">
+        <v>72</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9"/>
+      <c r="G9" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="30">
+        <v>566</v>
+      </c>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="M9"/>
+    </row>
+    <row r="10" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="14">
+        <v>45299</v>
+      </c>
+      <c r="C10" s="15">
+        <v>110</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10"/>
+      <c r="G10" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="31">
+        <v>460</v>
+      </c>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+    </row>
+    <row r="11" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="21">
+        <v>45300</v>
+      </c>
+      <c r="C11" s="22">
+        <v>81</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+    </row>
+    <row r="12" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="21">
+        <v>45301</v>
+      </c>
+      <c r="C12" s="22">
+        <v>105</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B13" s="21">
+        <v>45302</v>
+      </c>
+      <c r="C13" s="22">
+        <v>117</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="10"/>
+      <c r="G13"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B14" s="23">
+        <v>45303</v>
+      </c>
+      <c r="C14" s="24">
+        <v>101</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="10"/>
+      <c r="G14"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="25">
+        <v>45304</v>
+      </c>
+      <c r="C15" s="26">
+        <v>100</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="10"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="27">
+        <v>45305</v>
+      </c>
+      <c r="C16" s="28">
+        <v>53</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="10"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="27">
+        <v>45306</v>
+      </c>
+      <c r="C17" s="28">
+        <v>54</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="10"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="27">
+        <v>45307</v>
+      </c>
+      <c r="C18" s="28">
+        <v>62</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="27">
+        <v>45308</v>
+      </c>
+      <c r="C19" s="28">
+        <v>131</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="27">
+        <v>45309</v>
+      </c>
+      <c r="C20" s="28">
+        <v>132</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="27">
+        <v>45310</v>
+      </c>
+      <c r="C21" s="28">
+        <v>134</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="12">
+        <v>45311</v>
+      </c>
+      <c r="C22" s="18">
+        <v>75</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="1"/>
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="12">
+        <v>45312</v>
+      </c>
+      <c r="C23" s="18">
+        <v>84</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B24" s="12">
+        <v>45313</v>
+      </c>
+      <c r="C24" s="18">
+        <v>94</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B25" s="12">
+        <v>45314</v>
+      </c>
+      <c r="C25" s="18">
+        <v>102</v>
+      </c>
+      <c r="D25" s="9"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B26" s="19">
+        <v>45315</v>
+      </c>
+      <c r="C26" s="20">
+        <v>105</v>
+      </c>
+      <c r="D26" s="9"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B29" s="4" t="str" cm="1">
+        <f t="array" ref="B29:C36">_xlfn.DROP(
+    _xlfn.GROUPBY(
+        _xlfn.SCAN(0, C2:C25 &gt; C3:C26, _xleta.SUM),
+        B3:C26,
+        _xlfn.HSTACK(
+            _xlfn.LAMBDA(_xlpm.x, TEXT(_xlfn.SINGLE(_xlpm.x), "d/m/e") &amp; REPT(TEXT(MAX(_xlpm.x), "-d/m/e"), ROWS(_xlpm.x) &gt; 1)),
+            _xleta.SUM
+        ),
+        ,
+        0
+    ),
+    1,
+    1
+)</f>
+        <v>1/1/2024-3/1/2024</v>
+      </c>
+      <c r="C29">
+        <v>208</v>
+      </c>
+      <c r="E29" cm="1">
+        <f t="array" ref="E29:E52">_xlfn.SCAN(0, C2:C25 &gt; C3:C26, _xleta.SUM)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B30" s="4" t="str">
+        <v>4/1/2024</v>
+      </c>
+      <c r="C30">
+        <v>95</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B31" s="4" t="str">
+        <v>5/1/2024-8/1/2024</v>
+      </c>
+      <c r="C31">
+        <v>299</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B32" s="4" t="str">
+        <v>9/1/2024-11/1/2024</v>
+      </c>
+      <c r="C32">
+        <v>303</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B33" s="4" t="str">
+        <v>12/1/2024</v>
+      </c>
+      <c r="C33">
+        <v>101</v>
+      </c>
+      <c r="E33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B34" s="4" t="str">
+        <v>13/1/2024</v>
+      </c>
+      <c r="C34">
+        <v>100</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B35" s="4" t="str">
+        <v>14/1/2024-19/1/2024</v>
+      </c>
+      <c r="C35">
+        <v>566</v>
+      </c>
+      <c r="E35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B36" s="4" t="str">
+        <v>20/1/2024-24/1/2024</v>
+      </c>
+      <c r="C36">
+        <v>460</v>
+      </c>
+      <c r="E36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E41">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E42">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E43">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E44">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E46">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E47">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E48">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E49">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E50">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E51">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E52">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Still working through it
</commit_message>
<xml_diff>
--- a/CH-109 Custom Grouping.xlsx
+++ b/CH-109 Custom Grouping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FB31DC-61DC-4C0A-B44D-8687DCAF2F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288A3834-7842-4322-9727-C5781A0F6C7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1381,8 +1381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F6C4476-87DA-43D4-910A-472BFDC6FEAE}">
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1779,6 +1779,16 @@
         <v>105</v>
       </c>
       <c r="D26" s="9"/>
+      <c r="I26" t="str" cm="1">
+        <f t="array" ref="I26:K26">_xlfn.TEXTSPLIT(G29,",")</f>
+        <v>45292</v>
+      </c>
+      <c r="J26" t="str">
+        <v>45293</v>
+      </c>
+      <c r="K26" t="str">
+        <v>45294</v>
+      </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="str" cm="1">
@@ -1805,6 +1815,26 @@
         <f t="array" ref="E29:E52">_xlfn.SCAN(0, C2:C25 &gt; C3:C26, _xleta.SUM)</f>
         <v>1</v>
       </c>
+      <c r="G29" s="5" t="str" cm="1">
+        <f t="array" ref="G29:H36">_xlfn.DROP(
+    _xlfn.GROUPBY(
+        _xlfn.SCAN(0, C2:C25 &gt; C3:C26, _xleta.SUM),
+        B3:C26,
+        _xlfn.HSTACK(
+            _xlfn.LAMBDA(_xlpm.x, _xlfn.TEXTJOIN(",",TRUE,_xlpm.x)),
+            _xleta.SUM
+        ),
+        ,
+        0
+    ),
+    1,
+    1
+)</f>
+        <v>45292,45293,45294</v>
+      </c>
+      <c r="H29">
+        <v>208</v>
+      </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="str">
@@ -1816,6 +1846,12 @@
       <c r="E30">
         <v>1</v>
       </c>
+      <c r="G30" s="5" t="str">
+        <v>45295</v>
+      </c>
+      <c r="H30">
+        <v>95</v>
+      </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B31" s="4" t="str">
@@ -1827,6 +1863,12 @@
       <c r="E31">
         <v>1</v>
       </c>
+      <c r="G31" s="5" t="str">
+        <v>45296,45297,45298,45299</v>
+      </c>
+      <c r="H31">
+        <v>299</v>
+      </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B32" s="4" t="str">
@@ -1838,8 +1880,14 @@
       <c r="E32">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="G32" s="5" t="str">
+        <v>45300,45301,45302</v>
+      </c>
+      <c r="H32">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B33" s="4" t="str">
         <v>12/1/2024</v>
       </c>
@@ -1849,8 +1897,14 @@
       <c r="E33">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="G33" s="5" t="str">
+        <v>45303</v>
+      </c>
+      <c r="H33">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B34" s="4" t="str">
         <v>13/1/2024</v>
       </c>
@@ -1860,8 +1914,14 @@
       <c r="E34">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="G34" s="5" t="str">
+        <v>45304</v>
+      </c>
+      <c r="H34">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B35" s="4" t="str">
         <v>14/1/2024-19/1/2024</v>
       </c>
@@ -1871,8 +1931,14 @@
       <c r="E35">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="G35" s="5" t="str">
+        <v>45305,45306,45307,45308,45309,45310</v>
+      </c>
+      <c r="H35">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B36" s="4" t="str">
         <v>20/1/2024-24/1/2024</v>
       </c>
@@ -1882,63 +1948,69 @@
       <c r="E36">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="G36" s="5" t="str">
+        <v>45311,45312,45313,45314,45315</v>
+      </c>
+      <c r="H36">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E37">
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E38">
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E39">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E40">
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E41">
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E42">
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E43">
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E44">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E45">
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E46">
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E47">
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E48">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
I now understand it
</commit_message>
<xml_diff>
--- a/CH-109 Custom Grouping.xlsx
+++ b/CH-109 Custom Grouping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39DAA50-E066-4FE7-9655-81BF415A1CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316AFF41-0E44-4EB0-8BF1-5F08213872C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
   <si>
     <t>Question</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>https://www.linkedin.com/feed/update/urn:li:activity:7237927549903716352/</t>
+  </si>
+  <si>
+    <t>I now understand</t>
   </si>
 </sst>
 </file>
@@ -1382,7 +1385,7 @@
   <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1779,6 +1782,9 @@
         <v>105</v>
       </c>
       <c r="D26" s="9"/>
+      <c r="G26" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="I26" t="str" cm="1">
         <f t="array" ref="I26:K26">_xlfn.TEXTSPLIT(H29,",")</f>
         <v>47</v>

</xml_diff>

<commit_message>
I am going to play with this some more
</commit_message>
<xml_diff>
--- a/CH-109 Custom Grouping.xlsx
+++ b/CH-109 Custom Grouping.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316AFF41-0E44-4EB0-8BF1-5F08213872C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A86DEC-FFC3-418F-B8F0-7F3E3B5E0D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="Alt1" sheetId="2" r:id="rId2"/>
+    <sheet name="MySingleFunction" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Alt1'!$B$2:$D$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">MySingleFunction!$B$2:$D$26</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$D$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -63,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="13">
   <si>
     <t>Question</t>
   </si>
@@ -953,6 +955,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -1384,8 +1389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F6C4476-87DA-43D4-910A-472BFDC6FEAE}">
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView topLeftCell="A24" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2049,4 +2054,417 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CC4B8B1-1BD4-47DC-945B-242EC26D8BDD}">
+  <dimension ref="A1:N26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" customWidth="1"/>
+    <col min="4" max="5" width="12.21875" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" style="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="E1"/>
+      <c r="G1" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="35"/>
+      <c r="K1" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2"/>
+      <c r="G2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="16">
+        <v>45292</v>
+      </c>
+      <c r="C3" s="17">
+        <v>47</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3"/>
+      <c r="G3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="30">
+        <v>208</v>
+      </c>
+      <c r="I3" s="13"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="9"/>
+    </row>
+    <row r="4" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="16">
+        <v>45293</v>
+      </c>
+      <c r="C4" s="17">
+        <v>62</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4"/>
+      <c r="G4" s="12">
+        <v>45295</v>
+      </c>
+      <c r="H4" s="30">
+        <v>95</v>
+      </c>
+      <c r="I4" s="13"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="9"/>
+    </row>
+    <row r="5" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="16">
+        <v>45294</v>
+      </c>
+      <c r="C5" s="17">
+        <v>99</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5"/>
+      <c r="G5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="30">
+        <v>299</v>
+      </c>
+      <c r="I5" s="13"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="9"/>
+    </row>
+    <row r="6" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="12">
+        <v>45295</v>
+      </c>
+      <c r="C6" s="18">
+        <v>95</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6"/>
+      <c r="G6" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="30">
+        <v>303</v>
+      </c>
+      <c r="I6" s="13"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="9"/>
+    </row>
+    <row r="7" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="14">
+        <v>45296</v>
+      </c>
+      <c r="C7" s="15">
+        <v>52</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7"/>
+      <c r="G7" s="12">
+        <v>45303</v>
+      </c>
+      <c r="H7" s="30">
+        <v>101</v>
+      </c>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="14">
+        <v>45297</v>
+      </c>
+      <c r="C8" s="15">
+        <v>65</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8"/>
+      <c r="G8" s="12">
+        <v>45304</v>
+      </c>
+      <c r="H8" s="30">
+        <v>100</v>
+      </c>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+    </row>
+    <row r="9" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="14">
+        <v>45298</v>
+      </c>
+      <c r="C9" s="15">
+        <v>72</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9"/>
+      <c r="G9" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="30">
+        <v>566</v>
+      </c>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="M9"/>
+    </row>
+    <row r="10" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="14">
+        <v>45299</v>
+      </c>
+      <c r="C10" s="15">
+        <v>110</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10"/>
+      <c r="G10" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="31">
+        <v>460</v>
+      </c>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+    </row>
+    <row r="11" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="21">
+        <v>45300</v>
+      </c>
+      <c r="C11" s="22">
+        <v>81</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+    </row>
+    <row r="12" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="21">
+        <v>45301</v>
+      </c>
+      <c r="C12" s="22">
+        <v>105</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B13" s="21">
+        <v>45302</v>
+      </c>
+      <c r="C13" s="22">
+        <v>117</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="10"/>
+      <c r="G13"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B14" s="23">
+        <v>45303</v>
+      </c>
+      <c r="C14" s="24">
+        <v>101</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="10"/>
+      <c r="G14"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="25">
+        <v>45304</v>
+      </c>
+      <c r="C15" s="26">
+        <v>100</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="10"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="27">
+        <v>45305</v>
+      </c>
+      <c r="C16" s="28">
+        <v>53</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="10"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="27">
+        <v>45306</v>
+      </c>
+      <c r="C17" s="28">
+        <v>54</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="10"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="27">
+        <v>45307</v>
+      </c>
+      <c r="C18" s="28">
+        <v>62</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="27">
+        <v>45308</v>
+      </c>
+      <c r="C19" s="28">
+        <v>131</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="27">
+        <v>45309</v>
+      </c>
+      <c r="C20" s="28">
+        <v>132</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="27">
+        <v>45310</v>
+      </c>
+      <c r="C21" s="28">
+        <v>134</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="12">
+        <v>45311</v>
+      </c>
+      <c r="C22" s="18">
+        <v>75</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="1"/>
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="12">
+        <v>45312</v>
+      </c>
+      <c r="C23" s="18">
+        <v>84</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B24" s="12">
+        <v>45313</v>
+      </c>
+      <c r="C24" s="18">
+        <v>94</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B25" s="12">
+        <v>45314</v>
+      </c>
+      <c r="C25" s="18">
+        <v>102</v>
+      </c>
+      <c r="D25" s="9"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B26" s="19">
+        <v>45315</v>
+      </c>
+      <c r="C26" s="20">
+        <v>105</v>
+      </c>
+      <c r="D26" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Getting close to a model
</commit_message>
<xml_diff>
--- a/CH-109 Custom Grouping.xlsx
+++ b/CH-109 Custom Grouping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A86DEC-FFC3-418F-B8F0-7F3E3B5E0D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287DBAAD-5879-406B-9CF1-9030F04BDE9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="14">
   <si>
     <t>Question</t>
   </si>
@@ -105,11 +105,17 @@
   <si>
     <t>I now understand</t>
   </si>
+  <si>
+    <t>Try this as more of a model</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0;\-0;0;@"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -336,7 +342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -415,6 +421,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2058,10 +2065,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CC4B8B1-1BD4-47DC-945B-242EC26D8BDD}">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="D18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2072,6 +2079,8 @@
     <col min="4" max="5" width="12.21875" customWidth="1"/>
     <col min="6" max="6" width="19.88671875" customWidth="1"/>
     <col min="7" max="7" width="15.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2316,8 +2325,12 @@
         <v>117</v>
       </c>
       <c r="D13" s="9"/>
-      <c r="E13" s="10"/>
-      <c r="G13"/>
+      <c r="E13" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B14" s="23">
@@ -2339,7 +2352,25 @@
         <v>100</v>
       </c>
       <c r="D15" s="9"/>
-      <c r="E15" s="10"/>
+      <c r="E15" s="36" cm="1">
+        <f t="array" ref="E15:E38">_xlfn.SCAN(0, C2:C25 &gt; C3:C26, _xleta.SUM)</f>
+        <v>1</v>
+      </c>
+      <c r="F15" cm="1">
+        <f t="array" ref="F15:F22">_xlfn.UNIQUE(_xlfn.ANCHORARRAY(E15))</f>
+        <v>1</v>
+      </c>
+      <c r="G15" s="5" cm="1">
+        <f t="array" ref="G15:H17">_xlfn._xlws.FILTER(B3:C26,_xlfn.ANCHORARRAY(E15)=G13)</f>
+        <v>45292</v>
+      </c>
+      <c r="H15">
+        <v>47</v>
+      </c>
+      <c r="I15" t="str">
+        <f>TEXT(G15,"d/m/yyyy")&amp;REPT("-"&amp;TEXT(MAX(_xlfn.TAKE(_xlfn.ANCHORARRAY(G15),1,1)),"d/m/yyy")&amp;"|"&amp;SUM(_xlfn.TAKE(_xlfn.ANCHORARRAY(G15),,-1)),ROWS(_xlfn.ANCHORARRAY(G15))&gt;1)</f>
+        <v>1/1/2024-1/1/2024|208</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
@@ -2350,7 +2381,18 @@
         <v>53</v>
       </c>
       <c r="D16" s="9"/>
-      <c r="E16" s="10"/>
+      <c r="E16" s="36">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16" s="5">
+        <v>45293</v>
+      </c>
+      <c r="H16">
+        <v>62</v>
+      </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
@@ -2361,7 +2403,18 @@
         <v>54</v>
       </c>
       <c r="D17" s="9"/>
-      <c r="E17" s="10"/>
+      <c r="E17" s="36">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>3</v>
+      </c>
+      <c r="G17" s="5">
+        <v>45294</v>
+      </c>
+      <c r="H17">
+        <v>99</v>
+      </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
@@ -2372,7 +2425,12 @@
         <v>62</v>
       </c>
       <c r="D18" s="9"/>
-      <c r="E18" s="10"/>
+      <c r="E18" s="36">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>4</v>
+      </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
@@ -2383,7 +2441,12 @@
         <v>131</v>
       </c>
       <c r="D19" s="9"/>
-      <c r="E19" s="10"/>
+      <c r="E19" s="36">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>5</v>
+      </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
@@ -2394,7 +2457,12 @@
         <v>132</v>
       </c>
       <c r="D20" s="9"/>
-      <c r="E20" s="1"/>
+      <c r="E20" s="36">
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <v>6</v>
+      </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
@@ -2405,7 +2473,12 @@
         <v>134</v>
       </c>
       <c r="D21" s="9"/>
-      <c r="E21" s="1"/>
+      <c r="E21" s="36">
+        <v>3</v>
+      </c>
+      <c r="F21">
+        <v>7</v>
+      </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
@@ -2416,7 +2489,12 @@
         <v>75</v>
       </c>
       <c r="D22" s="9"/>
-      <c r="E22" s="1"/>
+      <c r="E22" s="36">
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <v>8</v>
+      </c>
       <c r="N22" s="2"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
@@ -2428,7 +2506,13 @@
         <v>84</v>
       </c>
       <c r="D23" s="9"/>
-      <c r="E23" s="1"/>
+      <c r="E23" s="36">
+        <v>4</v>
+      </c>
+      <c r="H23" t="str">
+        <f>I15</f>
+        <v>1/1/2024-1/1/2024|208</v>
+      </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B24" s="12">
@@ -2438,7 +2522,17 @@
         <v>94</v>
       </c>
       <c r="D24" s="9"/>
-      <c r="E24" s="1"/>
+      <c r="E24" s="36">
+        <v>4</v>
+      </c>
+      <c r="G24" s="5" cm="1">
+        <f t="array" ref="G24:G31">_xlfn.ANCHORARRAY(F15)</f>
+        <v>1</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="dataTable" ref="H24:H31" dt2D="0" dtr="0" r1="G13"/>
+        <v>1/1/2024-1/1/2024|208</v>
+      </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B25" s="12">
@@ -2448,7 +2542,15 @@
         <v>102</v>
       </c>
       <c r="D25" s="9"/>
-      <c r="E25" s="1"/>
+      <c r="E25" s="36">
+        <v>4</v>
+      </c>
+      <c r="G25" s="5">
+        <v>2</v>
+      </c>
+      <c r="H25" t="str">
+        <v>4/1/2024</v>
+      </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B26" s="19">
@@ -2458,6 +2560,105 @@
         <v>105</v>
       </c>
       <c r="D26" s="9"/>
+      <c r="E26" s="36">
+        <v>5</v>
+      </c>
+      <c r="G26" s="5">
+        <v>3</v>
+      </c>
+      <c r="H26" t="str">
+        <v>5/1/2024-5/1/2024|299</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E27" s="36">
+        <v>6</v>
+      </c>
+      <c r="G27" s="5">
+        <v>4</v>
+      </c>
+      <c r="H27" t="str">
+        <v>9/1/2024-9/1/2024|303</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E28" s="36">
+        <v>7</v>
+      </c>
+      <c r="G28" s="5">
+        <v>5</v>
+      </c>
+      <c r="H28" t="str">
+        <v>12/1/2024</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E29" s="36">
+        <v>7</v>
+      </c>
+      <c r="G29" s="5">
+        <v>6</v>
+      </c>
+      <c r="H29" t="str">
+        <v>13/1/2024</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E30" s="36">
+        <v>7</v>
+      </c>
+      <c r="G30" s="5">
+        <v>7</v>
+      </c>
+      <c r="H30" t="str">
+        <v>14/1/2024-14/1/2024|566</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E31" s="36">
+        <v>7</v>
+      </c>
+      <c r="G31" s="5">
+        <v>8</v>
+      </c>
+      <c r="H31" t="str">
+        <v>20/1/2024-20/1/2024|460</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E32" s="36">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E33" s="36">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E34" s="36">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E35" s="36">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E36" s="36">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E37" s="36">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E38" s="36">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Got my model done
</commit_message>
<xml_diff>
--- a/CH-109 Custom Grouping.xlsx
+++ b/CH-109 Custom Grouping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287DBAAD-5879-406B-9CF1-9030F04BDE9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5722CECB-6FD5-4637-BD60-FB5F839C77FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1397,7 +1397,7 @@
   <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView topLeftCell="A24" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2067,8 +2067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CC4B8B1-1BD4-47DC-945B-242EC26D8BDD}">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" topLeftCell="D12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2329,7 +2329,7 @@
         <v>13</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
@@ -2361,15 +2361,15 @@
         <v>1</v>
       </c>
       <c r="G15" s="5" cm="1">
-        <f t="array" ref="G15:H17">_xlfn._xlws.FILTER(B3:C26,_xlfn.ANCHORARRAY(E15)=G13)</f>
-        <v>45292</v>
+        <f t="array" ref="G15:H15">_xlfn._xlws.FILTER(B3:C26,_xlfn.ANCHORARRAY(E15)=G13)</f>
+        <v>45295</v>
       </c>
       <c r="H15">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="I15" t="str">
-        <f>TEXT(G15,"d/m/yyyy")&amp;REPT("-"&amp;TEXT(MAX(_xlfn.TAKE(_xlfn.ANCHORARRAY(G15),1,1)),"d/m/yyy")&amp;"|"&amp;SUM(_xlfn.TAKE(_xlfn.ANCHORARRAY(G15),,-1)),ROWS(_xlfn.ANCHORARRAY(G15))&gt;1)</f>
-        <v>1/1/2024-1/1/2024|208</v>
+        <f>IF(ROWS(_xlfn.ANCHORARRAY(G15))&gt;1,TEXT(G15,"d/m/yyyy")&amp;"-"&amp;TEXT(MAX(_xlfn.TAKE(_xlfn.ANCHORARRAY(G15),1,1)),"d/m/yyy")&amp;"|"&amp;SUM(_xlfn.TAKE(_xlfn.ANCHORARRAY(G15),,-1)),TEXT(G15,"d/m/yyyy")&amp;"|"&amp;SUM(_xlfn.TAKE(_xlfn.ANCHORARRAY(G15),,-1)))</f>
+        <v>4/1/2024|95</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
@@ -2387,12 +2387,6 @@
       <c r="F16">
         <v>2</v>
       </c>
-      <c r="G16" s="5">
-        <v>45293</v>
-      </c>
-      <c r="H16">
-        <v>62</v>
-      </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
@@ -2409,12 +2403,6 @@
       <c r="F17">
         <v>3</v>
       </c>
-      <c r="G17" s="5">
-        <v>45294</v>
-      </c>
-      <c r="H17">
-        <v>99</v>
-      </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
@@ -2511,7 +2499,7 @@
       </c>
       <c r="H23" t="str">
         <f>I15</f>
-        <v>1/1/2024-1/1/2024|208</v>
+        <v>4/1/2024|95</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
@@ -2533,6 +2521,13 @@
         <f t="dataTable" ref="H24:H31" dt2D="0" dtr="0" r1="G13"/>
         <v>1/1/2024-1/1/2024|208</v>
       </c>
+      <c r="K24" t="str" cm="1">
+        <f t="array" ref="K24:L31">_xlfn.DROP(_xlfn.REDUCE("",H24:H31,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.TEXTSPLIT(_xlpm.v,"|")))),1)</f>
+        <v>1/1/2024-1/1/2024</v>
+      </c>
+      <c r="L24" t="str">
+        <v>208</v>
+      </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B25" s="12">
@@ -2549,7 +2544,13 @@
         <v>2</v>
       </c>
       <c r="H25" t="str">
+        <v>4/1/2024|95</v>
+      </c>
+      <c r="K25" t="str">
         <v>4/1/2024</v>
+      </c>
+      <c r="L25" t="str">
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
@@ -2569,6 +2570,12 @@
       <c r="H26" t="str">
         <v>5/1/2024-5/1/2024|299</v>
       </c>
+      <c r="K26" t="str">
+        <v>5/1/2024-5/1/2024</v>
+      </c>
+      <c r="L26" t="str">
+        <v>299</v>
+      </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E27" s="36">
@@ -2580,6 +2587,12 @@
       <c r="H27" t="str">
         <v>9/1/2024-9/1/2024|303</v>
       </c>
+      <c r="K27" t="str">
+        <v>9/1/2024-9/1/2024</v>
+      </c>
+      <c r="L27" t="str">
+        <v>303</v>
+      </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E28" s="36">
@@ -2589,7 +2602,13 @@
         <v>5</v>
       </c>
       <c r="H28" t="str">
+        <v>12/1/2024|101</v>
+      </c>
+      <c r="K28" t="str">
         <v>12/1/2024</v>
+      </c>
+      <c r="L28" t="str">
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
@@ -2600,7 +2619,13 @@
         <v>6</v>
       </c>
       <c r="H29" t="str">
+        <v>13/1/2024|100</v>
+      </c>
+      <c r="K29" t="str">
         <v>13/1/2024</v>
+      </c>
+      <c r="L29" t="str">
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
@@ -2613,6 +2638,12 @@
       <c r="H30" t="str">
         <v>14/1/2024-14/1/2024|566</v>
       </c>
+      <c r="K30" t="str">
+        <v>14/1/2024-14/1/2024</v>
+      </c>
+      <c r="L30" t="str">
+        <v>566</v>
+      </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E31" s="36">
@@ -2623,6 +2654,12 @@
       </c>
       <c r="H31" t="str">
         <v>20/1/2024-20/1/2024|460</v>
+      </c>
+      <c r="K31" t="str">
+        <v>20/1/2024-20/1/2024</v>
+      </c>
+      <c r="L31" t="str">
+        <v>460</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Cleanup up some types
</commit_message>
<xml_diff>
--- a/CH-109 Custom Grouping.xlsx
+++ b/CH-109 Custom Grouping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5722CECB-6FD5-4637-BD60-FB5F839C77FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F146B0A1-B401-4BCE-AF0F-05C02BAFA906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2065,10 +2065,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CC4B8B1-1BD4-47DC-945B-242EC26D8BDD}">
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="F16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2081,6 +2081,7 @@
     <col min="7" max="7" width="15.88671875" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.6640625" customWidth="1"/>
     <col min="11" max="11" width="18.21875" customWidth="1"/>
+    <col min="13" max="13" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2368,8 +2369,8 @@
         <v>95</v>
       </c>
       <c r="I15" t="str">
-        <f>IF(ROWS(_xlfn.ANCHORARRAY(G15))&gt;1,TEXT(G15,"d/m/yyyy")&amp;"-"&amp;TEXT(MAX(_xlfn.TAKE(_xlfn.ANCHORARRAY(G15),1,1)),"d/m/yyy")&amp;"|"&amp;SUM(_xlfn.TAKE(_xlfn.ANCHORARRAY(G15),,-1)),TEXT(G15,"d/m/yyyy")&amp;"|"&amp;SUM(_xlfn.TAKE(_xlfn.ANCHORARRAY(G15),,-1)))</f>
-        <v>4/1/2024|95</v>
+        <f>IF(ROWS(_xlfn.ANCHORARRAY(G15))&gt;1,TEXT(G15,"d/m/yyyy")&amp;"-"&amp;TEXT(MAX(_xlfn.TAKE(_xlfn.ANCHORARRAY(G15),,1)),"d/m/yyy")&amp;"|"&amp;SUM(_xlfn.TAKE(_xlfn.ANCHORARRAY(G15),,-1)),TEXT(G15,"dd-mm-yyyy")&amp;"|"&amp;SUM(_xlfn.TAKE(_xlfn.ANCHORARRAY(G15),,-1)))</f>
+        <v>04-01-2024|95</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
@@ -2388,7 +2389,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="27">
         <v>45306</v>
@@ -2404,7 +2405,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="27">
         <v>45307</v>
@@ -2420,7 +2421,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="27">
         <v>45308</v>
@@ -2436,7 +2437,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="27">
         <v>45309</v>
@@ -2452,7 +2453,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="27">
         <v>45310</v>
@@ -2468,7 +2469,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="12">
         <v>45311</v>
@@ -2485,7 +2486,7 @@
       </c>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="12">
         <v>45312</v>
@@ -2499,10 +2500,10 @@
       </c>
       <c r="H23" t="str">
         <f>I15</f>
-        <v>4/1/2024|95</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+        <v>04-01-2024|95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B24" s="12">
         <v>45313</v>
       </c>
@@ -2519,17 +2520,32 @@
       </c>
       <c r="H24" t="str">
         <f t="dataTable" ref="H24:H31" dt2D="0" dtr="0" r1="G13"/>
-        <v>1/1/2024-1/1/2024|208</v>
+        <v>1/1/2024-3/1/2024|208</v>
       </c>
       <c r="K24" t="str" cm="1">
         <f t="array" ref="K24:L31">_xlfn.DROP(_xlfn.REDUCE("",H24:H31,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.TEXTSPLIT(_xlpm.v,"|")))),1)</f>
-        <v>1/1/2024-1/1/2024</v>
+        <v>1/1/2024-3/1/2024</v>
       </c>
       <c r="L24" t="str">
         <v>208</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M24" t="str" cm="1">
+        <f t="array" ref="M24:M31">K24:K31</f>
+        <v>1/1/2024-3/1/2024</v>
+      </c>
+      <c r="N24">
+        <f>L24+0</f>
+        <v>208</v>
+      </c>
+      <c r="O24" t="b" cm="1">
+        <f t="array" ref="O24:P31">M24:N31=G3:H10</f>
+        <v>1</v>
+      </c>
+      <c r="P24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B25" s="12">
         <v>45314</v>
       </c>
@@ -2544,16 +2560,29 @@
         <v>2</v>
       </c>
       <c r="H25" t="str">
-        <v>4/1/2024|95</v>
+        <v>04-01-2024|95</v>
       </c>
       <c r="K25" t="str">
-        <v>4/1/2024</v>
+        <v>04-01-2024</v>
       </c>
       <c r="L25" t="str">
         <v>95</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M25" t="str">
+        <v>04-01-2024</v>
+      </c>
+      <c r="N25">
+        <f t="shared" ref="N25:N31" si="0">L25+0</f>
+        <v>95</v>
+      </c>
+      <c r="O25" t="b">
+        <v>0</v>
+      </c>
+      <c r="P25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B26" s="19">
         <v>45315</v>
       </c>
@@ -2568,16 +2597,29 @@
         <v>3</v>
       </c>
       <c r="H26" t="str">
-        <v>5/1/2024-5/1/2024|299</v>
+        <v>5/1/2024-8/1/2024|299</v>
       </c>
       <c r="K26" t="str">
-        <v>5/1/2024-5/1/2024</v>
+        <v>5/1/2024-8/1/2024</v>
       </c>
       <c r="L26" t="str">
         <v>299</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M26" t="str">
+        <v>5/1/2024-8/1/2024</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="0"/>
+        <v>299</v>
+      </c>
+      <c r="O26" t="b">
+        <v>1</v>
+      </c>
+      <c r="P26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E27" s="36">
         <v>6</v>
       </c>
@@ -2585,16 +2627,29 @@
         <v>4</v>
       </c>
       <c r="H27" t="str">
-        <v>9/1/2024-9/1/2024|303</v>
+        <v>9/1/2024-11/1/2024|303</v>
       </c>
       <c r="K27" t="str">
-        <v>9/1/2024-9/1/2024</v>
+        <v>9/1/2024-11/1/2024</v>
       </c>
       <c r="L27" t="str">
         <v>303</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M27" t="str">
+        <v>9/1/2024-11/1/2024</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="0"/>
+        <v>303</v>
+      </c>
+      <c r="O27" t="b">
+        <v>1</v>
+      </c>
+      <c r="P27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E28" s="36">
         <v>7</v>
       </c>
@@ -2602,16 +2657,29 @@
         <v>5</v>
       </c>
       <c r="H28" t="str">
-        <v>12/1/2024|101</v>
+        <v>12-01-2024|101</v>
       </c>
       <c r="K28" t="str">
-        <v>12/1/2024</v>
+        <v>12-01-2024</v>
       </c>
       <c r="L28" t="str">
         <v>101</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M28" t="str">
+        <v>12-01-2024</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="0"/>
+        <v>101</v>
+      </c>
+      <c r="O28" t="b">
+        <v>0</v>
+      </c>
+      <c r="P28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E29" s="36">
         <v>7</v>
       </c>
@@ -2619,16 +2687,29 @@
         <v>6</v>
       </c>
       <c r="H29" t="str">
-        <v>13/1/2024|100</v>
+        <v>13-01-2024|100</v>
       </c>
       <c r="K29" t="str">
-        <v>13/1/2024</v>
+        <v>13-01-2024</v>
       </c>
       <c r="L29" t="str">
         <v>100</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M29" t="str">
+        <v>13-01-2024</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="O29" t="b">
+        <v>0</v>
+      </c>
+      <c r="P29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E30" s="36">
         <v>7</v>
       </c>
@@ -2636,16 +2717,29 @@
         <v>7</v>
       </c>
       <c r="H30" t="str">
-        <v>14/1/2024-14/1/2024|566</v>
+        <v>14/1/2024-19/1/2024|566</v>
       </c>
       <c r="K30" t="str">
-        <v>14/1/2024-14/1/2024</v>
+        <v>14/1/2024-19/1/2024</v>
       </c>
       <c r="L30" t="str">
         <v>566</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M30" t="str">
+        <v>14/1/2024-19/1/2024</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="0"/>
+        <v>566</v>
+      </c>
+      <c r="O30" t="b">
+        <v>1</v>
+      </c>
+      <c r="P30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E31" s="36">
         <v>7</v>
       </c>
@@ -2653,16 +2747,29 @@
         <v>8</v>
       </c>
       <c r="H31" t="str">
-        <v>20/1/2024-20/1/2024|460</v>
+        <v>20/1/2024-24/1/2024|460</v>
       </c>
       <c r="K31" t="str">
-        <v>20/1/2024-20/1/2024</v>
+        <v>20/1/2024-24/1/2024</v>
       </c>
       <c r="L31" t="str">
         <v>460</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M31" t="str">
+        <v>20/1/2024-24/1/2024</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="0"/>
+        <v>460</v>
+      </c>
+      <c r="O31" t="b">
+        <v>1</v>
+      </c>
+      <c r="P31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E32" s="36">
         <v>7</v>
       </c>

</xml_diff>